<commit_message>
Adding dashboard finishing touches
</commit_message>
<xml_diff>
--- a/Reference/Fleetpay Export 1_1_2025_1_32.xlsx
+++ b/Reference/Fleetpay Export 1_1_2025_1_32.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakew\OneDrive\Desktop\Code\fleetpay\Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D4F667-DD5A-4250-AF10-20E413E40148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E00AE1E-CE0B-4609-9196-76553D81D593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{D4EF7FA8-7B58-4662-92D1-106F6BF68379}"/>
+    <workbookView xWindow="340" yWindow="340" windowWidth="10800" windowHeight="18720" xr2:uid="{D4EF7FA8-7B58-4662-92D1-106F6BF68379}"/>
   </bookViews>
   <sheets>
     <sheet name="Fleetpay Export 1_1_2025_1_3" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="24">
   <si>
     <t>Project Number</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t xml:space="preserve">Avra Lavein </t>
+  </si>
+  <si>
+    <t>Jake Williams</t>
   </si>
 </sst>
 </file>
@@ -973,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D18B84-B996-4173-9089-19394B9216C1}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1676,6 +1679,132 @@
         <v>https://pf.apps.projectsforce.com/project/view/8430847</v>
       </c>
     </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>842020231</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="1">
+        <v>35</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" ref="F34:F39" si="0">HYPERLINK("https://pf.apps.projectsforce.com/project/view/8430847")</f>
+        <v>https://pf.apps.projectsforce.com/project/view/8430847</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>842020232</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="1">
+        <v>35</v>
+      </c>
+      <c r="E35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>https://pf.apps.projectsforce.com/project/view/8430847</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>842020233</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="1">
+        <v>35</v>
+      </c>
+      <c r="E36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>https://pf.apps.projectsforce.com/project/view/8430847</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>842020234</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="1">
+        <v>35</v>
+      </c>
+      <c r="E37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>https://pf.apps.projectsforce.com/project/view/8430847</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>842020235</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="1">
+        <v>35</v>
+      </c>
+      <c r="E38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>https://pf.apps.projectsforce.com/project/view/8430847</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>842020236</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="1">
+        <v>35</v>
+      </c>
+      <c r="E39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>https://pf.apps.projectsforce.com/project/view/8430847</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:F33">
     <sortCondition ref="B23:B33"/>

</xml_diff>